<commit_message>
Base de Datos/Copia de seguridad
Csvs de todas las tablas + Backup de la BD
</commit_message>
<xml_diff>
--- a/BD/src/main/resources/tablas/JuegosRol.xlsx
+++ b/BD/src/main/resources/tablas/JuegosRol.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="28515" windowHeight="12600"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="28515" windowHeight="12600" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="JuegosRol" sheetId="1" r:id="rId1"/>
@@ -12,17 +12,17 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="Ambientacion">JuegosRol!$P$2:$P$8</definedName>
-    <definedName name="Ambientación">JuegosRol!$P$2:$P$7</definedName>
-    <definedName name="Epoca">JuegosRol!$N$2:$N$5</definedName>
-    <definedName name="Época">JuegosRol!$N$2:$N$10</definedName>
+    <definedName name="Ambientacion">Hoja2!$C$2:$C$8</definedName>
+    <definedName name="Ambientación">Hoja2!$C$2:$C$7</definedName>
+    <definedName name="Epoca">Hoja2!$A$1:$A$4</definedName>
+    <definedName name="Época">Hoja2!$A$1:$A$9</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="37">
   <si>
     <t>20 aniversario</t>
   </si>
@@ -115,6 +115,24 @@
   </si>
   <si>
     <t>Época</t>
+  </si>
+  <si>
+    <t>Vampiro Edad Oscura</t>
+  </si>
+  <si>
+    <t>La llamada de Cthulhu</t>
+  </si>
+  <si>
+    <t>7ª Edición</t>
+  </si>
+  <si>
+    <t>Contemporaneo</t>
+  </si>
+  <si>
+    <t>Rol</t>
+  </si>
+  <si>
+    <t>D&amp;D3.5</t>
   </si>
 </sst>
 </file>
@@ -492,24 +510,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.5703125" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
-    <col min="14" max="14" width="15.85546875" customWidth="1"/>
-    <col min="15" max="15" width="13.85546875" customWidth="1"/>
-    <col min="16" max="16" width="23.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="13" max="13" width="15.85546875" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -517,13 +534,13 @@
         <v>29</v>
       </c>
       <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -531,19 +548,13 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -551,39 +562,27 @@
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -591,19 +590,13 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -611,19 +604,13 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -636,12 +623,8 @@
       <c r="D7" t="s">
         <v>24</v>
       </c>
-      <c r="N7" s="2"/>
-      <c r="P7" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -649,17 +632,13 @@
         <v>0</v>
       </c>
       <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
         <v>21</v>
       </c>
-      <c r="D8" t="s">
-        <v>25</v>
-      </c>
-      <c r="N8" s="2"/>
-      <c r="P8" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -667,15 +646,13 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
         <v>20</v>
       </c>
-      <c r="D9" t="s">
-        <v>27</v>
-      </c>
-      <c r="N9" s="2"/>
-      <c r="P9" s="3"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -683,15 +660,13 @@
         <v>0</v>
       </c>
       <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
         <v>21</v>
       </c>
-      <c r="D10" t="s">
-        <v>25</v>
-      </c>
-      <c r="N10" s="2"/>
-      <c r="P10" s="3"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -699,13 +674,13 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -713,27 +688,52 @@
         <v>0</v>
       </c>
       <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
         <v>21</v>
       </c>
-      <c r="D12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:B12">
     <sortCondition ref="A2:A12"/>
   </sortState>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C6 C8:C12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D6 D8:D12">
       <formula1>Ambientación</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7">
       <formula1>Ambientacion</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C12">
       <formula1>Época</formula1>
     </dataValidation>
   </dataValidations>
@@ -744,24 +744,316 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="23.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="C6" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="C7" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="C8" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" s="3"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576">
+      <formula1>Ambientacion</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>JuegosRol!$A$1:$A$14</xm:f>
+          </x14:formula1>
+          <xm:sqref>A1:A1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>